<commit_message>
New changes in some documentation
</commit_message>
<xml_diff>
--- a/Documentation/5.- Gestión del Proyecto/5.4.- Métricas del Producto y Estimaciones/1.- Métricas y estimaciones.xlsx
+++ b/Documentation/5.- Gestión del Proyecto/5.4.- Métricas del Producto y Estimaciones/1.- Métricas y estimaciones.xlsx
@@ -1058,9 +1058,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:from>
     <xdr:ext cy="3048000" cx="4286250"/>
     <xdr:graphicFrame>
@@ -1312,7 +1312,7 @@
         <v>16</v>
       </c>
       <c s="5" r="C15">
-        <v>13</v>
+        <v>28.99</v>
       </c>
       <c s="3" r="D15"/>
     </row>
@@ -1322,7 +1322,7 @@
         <v>6</v>
       </c>
       <c s="5" r="C16">
-        <v>23</v>
+        <v>46.83</v>
       </c>
       <c s="3" r="D16"/>
     </row>
@@ -1332,7 +1332,7 @@
         <v>17</v>
       </c>
       <c s="5" r="C17">
-        <v>34</v>
+        <v>84.74</v>
       </c>
       <c s="3" r="D17"/>
     </row>
@@ -1342,7 +1342,7 @@
         <v>8</v>
       </c>
       <c s="5" r="C18">
-        <v>35</v>
+        <v>75.82</v>
       </c>
       <c s="3" r="D18"/>
     </row>
@@ -1352,7 +1352,7 @@
         <v>18</v>
       </c>
       <c s="5" r="C19">
-        <v>19</v>
+        <v>78.05</v>
       </c>
       <c s="3" r="D19"/>
     </row>
@@ -1398,21 +1398,21 @@
         <v>6</v>
       </c>
       <c s="5" r="C24">
-        <v>23</v>
+        <v>46.83</v>
       </c>
       <c s="7" r="D24">
         <v>3050</v>
       </c>
       <c s="6" r="E24">
         <f>D24/C24</f>
-        <v>132.608695652174</v>
+        <v>65.1291906897288</v>
       </c>
       <c s="5" r="F24">
         <v>1</v>
       </c>
       <c s="5" r="G24">
         <f>(D24/E24)*F24</f>
-        <v>23</v>
+        <v>46.83</v>
       </c>
       <c s="2" r="H24"/>
     </row>
@@ -1422,7 +1422,7 @@
         <v>17</v>
       </c>
       <c s="5" r="C25">
-        <v>34</v>
+        <v>84.74</v>
       </c>
       <c s="7" r="D25">
         <f>2218+608</f>
@@ -1430,14 +1430,14 @@
       </c>
       <c s="6" r="E25">
         <f>D25/C25</f>
-        <v>83.1176470588235</v>
+        <v>33.3490677366061</v>
       </c>
       <c s="5" r="F25">
         <v>1.3</v>
       </c>
       <c s="5" r="G25">
         <f>(D25/E25)*F25</f>
-        <v>44.2</v>
+        <v>110.162</v>
       </c>
       <c s="2" r="H25"/>
     </row>
@@ -1447,21 +1447,21 @@
         <v>8</v>
       </c>
       <c s="5" r="C26">
-        <v>35</v>
+        <v>75.82</v>
       </c>
       <c s="7" r="D26">
         <v>2052</v>
       </c>
       <c s="6" r="E26">
         <f>D26/C26</f>
-        <v>58.6285714285714</v>
+        <v>27.0640991822738</v>
       </c>
       <c s="5" r="F26">
         <v>1.3</v>
       </c>
       <c s="5" r="G26">
         <f>(D26/E26)*F26</f>
-        <v>45.5</v>
+        <v>98.566</v>
       </c>
       <c s="2" r="H26"/>
       <c s="14" r="P26"/>
@@ -1474,8 +1474,7 @@
         <v>18</v>
       </c>
       <c s="5" r="C27">
-        <f>19+13</f>
-        <v>32</v>
+        <v>107.04</v>
       </c>
       <c s="7" r="D27">
         <f>48+1067</f>
@@ -1483,14 +1482,14 @@
       </c>
       <c s="6" r="E27">
         <f>D27/C27</f>
-        <v>34.84375</v>
+        <v>10.4166666666667</v>
       </c>
       <c s="5" r="F27">
         <v>1.2</v>
       </c>
       <c s="5" r="G27">
         <f>(D27/E27)*F27</f>
-        <v>38.4</v>
+        <v>128.448</v>
       </c>
       <c s="2" r="H27"/>
       <c s="10" r="P27"/>

</xml_diff>